<commit_message>
work on analysis for the paper, re-run figures
</commit_message>
<xml_diff>
--- a/output_for_paper/SBS.table.xlsx
+++ b/output_for_paper/SBS.table.xlsx
@@ -1,82 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\non-M\github\mSigHdp_paper_sup_files_x1\output_for_paper\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5A7BD9-2198-47FA-A2FE-0039E0E8D054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-38510" yWindow="-10960" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SBS" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="SBS" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t xml:space="preserve">Composite measure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+  <si>
+    <t>Composite measure</t>
+  </si>
+  <si>
+    <t>Data
 set</t>
   </si>
   <si>
-    <t xml:space="preserve">Approach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Mean
 PPV</t>
   </si>
   <si>
-    <t xml:space="preserve">Mean
+    <t>Mean
 TPR</t>
   </si>
   <si>
-    <t xml:space="preserve">Mean cosine
+    <t>Mean cosine
 similarity</t>
   </si>
   <si>
-    <t xml:space="preserve">SBS_set1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mSigHdp_ds_3k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mSigHdp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SigProfilerExtractor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NR_hdp_gb_20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NR_hdp_gb_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">signeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SignatureAnalyzer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBS_set2</t>
+    <t>SBS_set1</t>
+  </si>
+  <si>
+    <t>mSigHdp_ds_3k</t>
+  </si>
+  <si>
+    <t>mSigHdp</t>
+  </si>
+  <si>
+    <t>SigProfilerExtractor</t>
+  </si>
+  <si>
+    <t>NR_hdp_gb_20</t>
+  </si>
+  <si>
+    <t>NR_hdp_gb_1</t>
+  </si>
+  <si>
+    <t>signeR</t>
+  </si>
+  <si>
+    <t>SignatureAnalyzer</t>
+  </si>
+  <si>
+    <t>SBS_set2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00"/>
-  </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -90,10 +95,10 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,36 +118,56 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -424,20 +449,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2">
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -460,313 +494,313 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>2.86964381694272</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0.0361738489782219</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0.990909090909091</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>0.88695652173913</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>0.991778204294496</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="1">
+        <v>2.8696438169427201</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.6173848978221901E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.99090909090909096</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.88695652173912998</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.99177820429449604</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>2.63385704521021</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0.025316398928073</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>0.775840455840456</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>0.869565217391304</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>0.988451371978451</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="C4" s="1">
+        <v>2.6338570452102101</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.5316398928073001E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.77584045584045602</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.86956521739130399</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.98845137197845101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="1">
         <v>2.62076494242991</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>0.039071081348171</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0.941748366013072</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>0.704347826086956</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>0.974668750329883</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="D5" s="1">
+        <v>3.9071081348171E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.94174836601307199</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.70434782608695601</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.97466875032988298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>2.45005584837433</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0.0359857139003561</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>0.535226183031061</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>0.930434782608696</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>0.984394882734575</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="C6" s="1">
+        <v>2.4500558483743302</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.5985713900356098E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.53522618303106095</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.93043478260869605</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.98439488273457498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>2.38703026494603</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>0.0724233090864231</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>0.445003817129689</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>0.956521739130435</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>0.985504708685903</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="C7" s="1">
+        <v>2.3870302649460302</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.2423309086423096E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.44500381712968901</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.95652173913043503</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.98550470868590301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="n">
-        <v>2.26262175089725</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>0.127518458492113</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>0.560454002389486</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>0.721739130434783</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>0.98042861807298</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="C8" s="1">
+        <v>2.2626217508972499</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.12751845849211299</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.56045400238948595</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.72173913043478299</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.98042861807297998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="n">
-        <v>1.83879010302383</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>0.0590465430415345</v>
-      </c>
-      <c r="E9" s="1" t="n">
+      <c r="C9" s="1">
+        <v>1.8387901030238301</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5.9046543041534498E-2</v>
+      </c>
+      <c r="E9" s="1">
         <v>0.291304347826087</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>0.582608695652174</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>0.964877059545565</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="F9" s="1">
+        <v>0.58260869565217399</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.96487705954556502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="n">
-        <v>2.66650310981278</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>0.0227478583077535</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>0.899357220046875</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>0.775</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>0.992145889765905</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="C10" s="1">
+        <v>2.6665031098127798</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2.2747858307753499E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.89935722004687502</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.99214588976590501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="n">
-        <v>2.51573176164722</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>0.0320518470209052</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>0.725564462627156</v>
-      </c>
-      <c r="F11" s="1" t="n">
+      <c r="C11" s="1">
+        <v>2.5157317616472201</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3.2051847020905203E-2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.72556446262715601</v>
+      </c>
+      <c r="F11" s="1">
         <v>0.8</v>
       </c>
-      <c r="G11" s="1" t="n">
-        <v>0.990167299020063</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="G11" s="1">
+        <v>0.99016729902006295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="n">
-        <v>2.36770138181721</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>0.045297983436451</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>0.531320754716981</v>
-      </c>
-      <c r="F12" s="1" t="n">
+      <c r="C12" s="1">
+        <v>2.3677013818172101</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4.5297983436451E-2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.53132075471698104</v>
+      </c>
+      <c r="F12" s="1">
         <v>0.85</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="G12" s="1">
         <v>0.986380627100229</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="n">
-        <v>2.24731755637892</v>
-      </c>
-      <c r="D13" s="1" t="n">
+      <c r="C13" s="1">
+        <v>2.2473175563789201</v>
+      </c>
+      <c r="D13" s="1">
         <v>0.121053353629316</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="1">
         <v>0.895299145299145</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>0.3875</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>0.964518411079777</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="F13" s="1">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.96451841107977698</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>2.07081907525817</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>0.0824169433012825</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>0.57701888915682</v>
-      </c>
-      <c r="F14" s="1" t="n">
-        <v>0.5125</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>0.981300186101349</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="C14" s="1">
+        <v>2.0708190752581701</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8.2416943301282505E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.57701888915681998</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.51249999999999996</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.98130018610134895</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1" t="n">
-        <v>1.53699734037393</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>0.0323609713798259</v>
-      </c>
-      <c r="E15" s="1" t="n">
+      <c r="C15" s="1">
+        <v>1.5369973403739301</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3.2360971379825902E-2</v>
+      </c>
+      <c r="E15" s="1">
         <v>0.191705069124424</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="1">
         <v>0.375</v>
       </c>
-      <c r="G15" s="1" t="n">
-        <v>0.970292271249508</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G15" s="1">
+        <v>0.97029227124950801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -775,6 +809,6 @@
     <mergeCell ref="A10:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated summary table and plots
</commit_message>
<xml_diff>
--- a/output_for_paper/SBS.table.xlsx
+++ b/output_for_paper/SBS.table.xlsx
@@ -1,87 +1,82 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\non-M\github\mSigHdp_paper_sup_files_x1\output_for_paper\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5A7BD9-2198-47FA-A2FE-0039E0E8D054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-10960" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="SBS" sheetId="1" r:id="rId1"/>
+    <sheet name="SBS" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
-  <si>
-    <t>Composite measure</t>
-  </si>
-  <si>
-    <t>Data
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t xml:space="preserve">Composite measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data
 set</t>
   </si>
   <si>
-    <t>Approach</t>
-  </si>
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>Mean
+    <t xml:space="preserve">Approach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean
 PPV</t>
   </si>
   <si>
-    <t>Mean
+    <t xml:space="preserve">Mean
 TPR</t>
   </si>
   <si>
-    <t>Mean cosine
+    <t xml:space="preserve">Mean cosine
 similarity</t>
   </si>
   <si>
-    <t>SBS_set1</t>
-  </si>
-  <si>
-    <t>mSigHdp_ds_3k</t>
-  </si>
-  <si>
-    <t>mSigHdp</t>
-  </si>
-  <si>
-    <t>SigProfilerExtractor</t>
-  </si>
-  <si>
-    <t>NR_hdp_gb_20</t>
-  </si>
-  <si>
-    <t>NR_hdp_gb_1</t>
-  </si>
-  <si>
-    <t>signeR</t>
-  </si>
-  <si>
-    <t>SignatureAnalyzer</t>
-  </si>
-  <si>
-    <t>SBS_set2</t>
+    <t xml:space="preserve">SBS_set1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mSigHdp_ds_3k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mSigHdp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SigProfilerExtractor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NR_hdp_gb_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NR_hdp_gb_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signeR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SignatureAnalyzer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBS_set2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.00"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,10 +90,10 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,56 +113,36 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -449,29 +424,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C1" s="4" t="s">
+    <row r="1">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -494,313 +460,313 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
-        <v>2.8696438169427201</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3.6173848978221901E-2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.99090909090909096</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.88695652173912998</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.99177820429449604</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="C3" s="1" t="n">
+        <v>2.87542938981382</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0.0353224432988468</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0.992424242424242</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0.891304347826087</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.991700799563489</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1">
-        <v>2.6338570452102101</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2.5316398928073001E-2</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.77584045584045602</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.86956521739130399</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.98845137197845101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="C4" s="1" t="n">
+        <v>2.63385704521021</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.025316398928073</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0.775840455840456</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.869565217391304</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.988451371978451</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>2.62076494242991</v>
       </c>
-      <c r="D5" s="1">
-        <v>3.9071081348171E-2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.94174836601307199</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.70434782608695601</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.97466875032988298</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="D5" s="1" t="n">
+        <v>0.039071081348171</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.941748366013072</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.704347826086956</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0.974668750329883</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
-        <v>2.4500558483743302</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3.5985713900356098E-2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.53522618303106095</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.93043478260869605</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.98439488273457498</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="C6" s="1" t="n">
+        <v>2.45005584837433</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0.0359857139003561</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0.535226183031061</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.930434782608696</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0.984394882734575</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1">
-        <v>2.3870302649460302</v>
-      </c>
-      <c r="D7" s="1">
-        <v>7.2423309086423096E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.44500381712968901</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.95652173913043503</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.98550470868590301</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="C7" s="1" t="n">
+        <v>2.38703026494603</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0.0724233090864231</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0.445003817129689</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0.956521739130435</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0.985504708685903</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1">
-        <v>2.2626217508972499</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.12751845849211299</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.56045400238948595</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.72173913043478299</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.98042861807297998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="C8" s="1" t="n">
+        <v>2.293532762121</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0.0546863916049356</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0.592596153846154</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0.721739130434783</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0.979197477840062</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1">
-        <v>1.8387901030238301</v>
-      </c>
-      <c r="D9" s="1">
-        <v>5.9046543041534498E-2</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="C9" s="1" t="n">
+        <v>1.83879010302383</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0.0590465430415345</v>
+      </c>
+      <c r="E9" s="1" t="n">
         <v>0.291304347826087</v>
       </c>
-      <c r="F9" s="1">
-        <v>0.58260869565217399</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.96487705954556502</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="F9" s="1" t="n">
+        <v>0.582608695652174</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>0.964877059545565</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1">
-        <v>2.6665031098127798</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2.2747858307753499E-2</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.89935722004687502</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.99214588976590501</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="C10" s="1" t="n">
+        <v>2.66650310981278</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0.0227478583077535</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0.899357220046875</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>0.992145889765905</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1">
-        <v>2.5157317616472201</v>
-      </c>
-      <c r="D11" s="1">
-        <v>3.2051847020905203E-2</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.72556446262715601</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="C11" s="1" t="n">
+        <v>2.51573176164722</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0.0320518470209052</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>0.725564462627156</v>
+      </c>
+      <c r="F11" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="G11" s="1">
-        <v>0.99016729902006295</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="G11" s="1" t="n">
+        <v>0.990167299020063</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1">
-        <v>2.3677013818172101</v>
-      </c>
-      <c r="D12" s="1">
-        <v>4.5297983436451E-2</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.53132075471698104</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="C12" s="1" t="n">
+        <v>2.36770138181721</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0.045297983436451</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>0.531320754716981</v>
+      </c>
+      <c r="F12" s="1" t="n">
         <v>0.85</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="1" t="n">
         <v>0.986380627100229</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="13">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1">
-        <v>2.2473175563789201</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="1" t="n">
+        <v>2.24731755637892</v>
+      </c>
+      <c r="D13" s="1" t="n">
         <v>0.121053353629316</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="1" t="n">
         <v>0.895299145299145</v>
       </c>
-      <c r="F13" s="1">
-        <v>0.38750000000000001</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0.96451841107977698</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="F13" s="1" t="n">
+        <v>0.3875</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>0.964518411079777</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1">
-        <v>2.0708190752581701</v>
-      </c>
-      <c r="D14" s="1">
-        <v>8.2416943301282505E-2</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.57701888915681998</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0.51249999999999996</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0.98130018610134895</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="C14" s="1" t="n">
+        <v>2.07081907525817</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0.0824169433012825</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>0.57701888915682</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>0.5125</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>0.981300186101349</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1">
-        <v>1.5369973403739301</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3.2360971379825902E-2</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="C15" s="1" t="n">
+        <v>1.53699734037393</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0.0323609713798259</v>
+      </c>
+      <c r="E15" s="1" t="n">
         <v>0.191705069124424</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="1" t="n">
         <v>0.375</v>
       </c>
-      <c r="G15" s="1">
-        <v>0.97029227124950801</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="G15" s="1" t="n">
+        <v>0.970292271249508</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -809,6 +775,6 @@
     <mergeCell ref="A10:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
renamed Realistic to tmp_Realistic for SP_default; deleted old intermediate files
</commit_message>
<xml_diff>
--- a/output_for_paper/SBS.table.xlsx
+++ b/output_for_paper/SBS.table.xlsx
@@ -586,19 +586,19 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>2.293532762121</v>
+        <v>2.31244962562356</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0.0546863916049356</v>
+        <v>0.0948663428343971</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>0.592596153846154</v>
+        <v>0.577820197044335</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0.721739130434783</v>
+        <v>0.756521739130435</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>0.979197477840062</v>
+        <v>0.978107689448793</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
added new wilcoxon test and stats for sensitivity
</commit_message>
<xml_diff>
--- a/output_for_paper/SBS.table.xlsx
+++ b/output_for_paper/SBS.table.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Composite Measure</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t xml:space="preserve">Wilcoxon rank-sum test mSigHdp_ds_3k vs SigProfilerExtractor p = 3.248e-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilcoxon rank-sum test mSigHdp_ds_3k vs mSigHdp p = 4.33e-05</t>
   </si>
 </sst>
 </file>
@@ -776,6 +779,11 @@
         <v>17</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C1:D1"/>

</xml_diff>

<commit_message>
Added NR_hdp_gb_1 results on SBS_set2/Realistic to summary tables and summary plots
</commit_message>
<xml_diff>
--- a/output_for_paper/SBS.table.xlsx
+++ b/output_for_paper/SBS.table.xlsx
@@ -724,22 +724,22 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>2.07081907525817</v>
+        <v>2.19707955583194</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.0824169433012825</v>
+        <v>0.0773183260467158</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>0.57701888915682</v>
+        <v>0.319131092406954</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>0.5125</v>
+        <v>0.89375</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.981300186101349</v>
+        <v>0.984198463424988</v>
       </c>
     </row>
     <row r="15">
@@ -747,40 +747,63 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>2.07081907525817</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0.0824169433012825</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>0.57701888915682</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>0.5125</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>0.981300186101349</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C16" s="1" t="n">
         <v>1.53699734037393</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D16" s="1" t="n">
         <v>0.0323609713798259</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E16" s="1" t="n">
         <v>0.191705069124424</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F16" s="1" t="n">
         <v>0.375</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="G16" s="1" t="n">
         <v>0.970292271249508</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
@@ -788,7 +811,7 @@
   <mergeCells count="3">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A10:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>